<commit_message>
update name logic, update controller summary, logic t upload file, get file, get avatar
</commit_message>
<xml_diff>
--- a/API/Templates/Student_Import_Template.xlsx
+++ b/API/Templates/Student_Import_Template.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myFolder-CUSTOME\code_place\Capstone_Resolvemaster\API\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7034D9-4D01-467B-981D-E3564D071216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CD9FF8-4F12-4A19-84EE-469859DCFC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{057623EF-F0A2-4C22-BAD6-956A92D5D57E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="School" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,20 +37,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Gmail</t>
   </si>
   <si>
-    <t>Date of birth (dd/MM/yyyy)</t>
-  </si>
-  <si>
     <t>EIU's Student Import Template</t>
   </si>
   <si>
-    <t>Full Name</t>
-  </si>
-  <si>
     <t>Order</t>
   </si>
   <si>
@@ -57,6 +52,21 @@
   </si>
   <si>
     <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>First  Name</t>
+  </si>
+  <si>
+    <t>Las tName</t>
   </si>
 </sst>
 </file>
@@ -89,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -112,20 +122,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,7 +505,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -473,39 +515,40 @@
     <col min="4" max="4" width="22.8984375" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="22.796875" customWidth="1"/>
+    <col min="7" max="7" width="13.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
+      <c r="A5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -514,4 +557,32 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FFE7972-6DD9-40C3-BA73-BB8D22F323B4}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>